<commit_message>
Substituindo login e cadastro por um modal
</commit_message>
<xml_diff>
--- a/Planilha de backlog.xlsx
+++ b/Planilha de backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TUCO\Desktop\projeto react\projeto-react\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E96553D-F8CC-4D48-B4E7-62953F2A0279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2775D05-5B2F-48ED-9BB3-325D2D2024E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9A0F8931-611D-4554-9C7E-254CD5D85667}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="54">
   <si>
     <t>Criação da pag inicial</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>Criação da dropbox</t>
+  </si>
+  <si>
+    <t>Modelagem do banco de Dados</t>
+  </si>
+  <si>
+    <t>Modelagem</t>
   </si>
 </sst>
 </file>
@@ -538,20 +544,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86938D1B-0EAC-44A7-BB9A-D44CCB9B87B8}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="14.5546875" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
     <col min="5" max="5" width="17.21875" customWidth="1"/>
     <col min="6" max="6" width="12.109375" customWidth="1"/>
     <col min="7" max="7" width="12.5546875" customWidth="1"/>
-    <col min="8" max="9" width="14.77734375" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.5">
@@ -604,10 +611,10 @@
         <v>13</v>
       </c>
       <c r="H2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.5">
@@ -631,10 +638,10 @@
         <v>8</v>
       </c>
       <c r="H3" s="2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.5">
@@ -658,10 +665,10 @@
         <v>8</v>
       </c>
       <c r="H4" s="2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.5">
@@ -685,10 +692,10 @@
         <v>21</v>
       </c>
       <c r="H5" s="2">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.5">
@@ -791,10 +798,10 @@
         <v>3</v>
       </c>
       <c r="H9" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.5">
@@ -816,10 +823,10 @@
         <v>3</v>
       </c>
       <c r="H10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.5">
@@ -866,10 +873,10 @@
         <v>13</v>
       </c>
       <c r="H12" s="2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I12" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.5">
@@ -916,10 +923,10 @@
         <v>8</v>
       </c>
       <c r="H14" s="2">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I14" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.5">
@@ -1064,7 +1071,9 @@
       <c r="B20" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="1">
+        <v>30</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20" t="s">
         <v>33</v>
@@ -1089,7 +1098,9 @@
       <c r="B21" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="1"/>
+      <c r="C21" s="1">
+        <v>21</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" t="s">
         <v>36</v>
@@ -1336,17 +1347,36 @@
         <v>5</v>
       </c>
       <c r="H30" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="I30" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A31" s="1"/>
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="H31" s="2"/>
+      <c r="E31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31">
+        <v>8</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0</v>
+      </c>
+      <c r="I31" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:I31">

</xml_diff>